<commit_message>
Stocks prices are now scraped with multiple threads at once
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -394,7 +394,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1365"/>
+  <dimension ref="A1:L1368"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1240" activePane="bottomRight" state="frozenSplit"/>
@@ -45681,6 +45681,126 @@
         <v>3025</v>
       </c>
     </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>2022-12-25</t>
+        </is>
+      </c>
+      <c r="B1366" t="n">
+        <v>62580.5</v>
+      </c>
+      <c r="C1366" t="n">
+        <v>-4506</v>
+      </c>
+      <c r="D1366" t="n">
+        <v>53339</v>
+      </c>
+      <c r="E1366" t="n">
+        <v>48833</v>
+      </c>
+      <c r="F1366" t="n">
+        <v>111413.5</v>
+      </c>
+      <c r="G1366" t="n">
+        <v>71669</v>
+      </c>
+      <c r="H1366" t="n">
+        <v>186107.5</v>
+      </c>
+      <c r="I1366" t="n">
+        <v>43.39</v>
+      </c>
+      <c r="J1366" t="n">
+        <v>-1658</v>
+      </c>
+      <c r="K1366" t="n">
+        <v>11728.28</v>
+      </c>
+      <c r="L1366" t="n">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>2022-12-26</t>
+        </is>
+      </c>
+      <c r="B1367" t="n">
+        <v>62580.5</v>
+      </c>
+      <c r="C1367" t="n">
+        <v>-4506</v>
+      </c>
+      <c r="D1367" t="n">
+        <v>53921</v>
+      </c>
+      <c r="E1367" t="n">
+        <v>49415</v>
+      </c>
+      <c r="F1367" t="n">
+        <v>111995.5</v>
+      </c>
+      <c r="G1367" t="n">
+        <v>71669</v>
+      </c>
+      <c r="H1367" t="n">
+        <v>186689.5</v>
+      </c>
+      <c r="I1367" t="n">
+        <v>43.39</v>
+      </c>
+      <c r="J1367" t="n">
+        <v>-1655</v>
+      </c>
+      <c r="K1367" t="n">
+        <v>12194.38</v>
+      </c>
+      <c r="L1367" t="n">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>2022-12-30</t>
+        </is>
+      </c>
+      <c r="B1368" t="n">
+        <v>62580.5</v>
+      </c>
+      <c r="C1368" t="n">
+        <v>-4442</v>
+      </c>
+      <c r="D1368" t="n">
+        <v>52724</v>
+      </c>
+      <c r="E1368" t="n">
+        <v>48282</v>
+      </c>
+      <c r="F1368" t="n">
+        <v>110862.5</v>
+      </c>
+      <c r="G1368" t="n">
+        <v>71607</v>
+      </c>
+      <c r="H1368" t="n">
+        <v>185464.5</v>
+      </c>
+      <c r="I1368" t="n">
+        <v>43.39</v>
+      </c>
+      <c r="J1368" t="n">
+        <v>-1668</v>
+      </c>
+      <c r="K1368" t="n">
+        <v>11873.16</v>
+      </c>
+      <c r="L1368" t="n">
+        <v>2995</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>

<commit_message>
nr update and clean up
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -394,7 +394,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1368"/>
+  <dimension ref="A1:L1369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1240" activePane="bottomRight" state="frozenSplit"/>
@@ -45801,6 +45801,46 @@
         <v>2995</v>
       </c>
     </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>2022-12-31</t>
+        </is>
+      </c>
+      <c r="B1369" t="n">
+        <v>62580.5</v>
+      </c>
+      <c r="C1369" t="n">
+        <v>-4442</v>
+      </c>
+      <c r="D1369" t="n">
+        <v>53034</v>
+      </c>
+      <c r="E1369" t="n">
+        <v>48592</v>
+      </c>
+      <c r="F1369" t="n">
+        <v>111172.5</v>
+      </c>
+      <c r="G1369" t="n">
+        <v>71519</v>
+      </c>
+      <c r="H1369" t="n">
+        <v>185446.5</v>
+      </c>
+      <c r="I1369" t="n">
+        <v>43.39</v>
+      </c>
+      <c r="J1369" t="n">
+        <v>-1654</v>
+      </c>
+      <c r="K1369" t="n">
+        <v>11847.88</v>
+      </c>
+      <c r="L1369" t="n">
+        <v>2755</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>

<commit_message>
formatting and req changes, so it runs on vs code more easily
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -51585,31 +51585,31 @@
         <v>-4189</v>
       </c>
       <c r="D1437" t="n">
-        <v>66993</v>
+        <v>66994</v>
       </c>
       <c r="E1437" t="n">
-        <v>62804</v>
+        <v>62805</v>
       </c>
       <c r="F1437" t="n">
-        <v>136010</v>
+        <v>136011</v>
       </c>
       <c r="G1437" t="n">
         <v>79972</v>
       </c>
       <c r="H1437" t="n">
-        <v>220972</v>
+        <v>220974</v>
       </c>
       <c r="I1437" t="n">
         <v>72.95</v>
       </c>
       <c r="J1437" t="n">
-        <v>-383</v>
+        <v>-382</v>
       </c>
       <c r="K1437" t="n">
         <v>10025.48</v>
       </c>
       <c r="L1437" t="n">
-        <v>4990</v>
+        <v>4991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Funderbeam commented out bc of 2FA
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -394,7 +394,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1449"/>
+  <dimension ref="A1:L1450"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1004" activePane="bottomRight" state="frozenSplit"/>
@@ -52092,6 +52092,46 @@
         <v>5000</v>
       </c>
     </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>2023-08-26</t>
+        </is>
+      </c>
+      <c r="B1450" t="n">
+        <v>78240</v>
+      </c>
+      <c r="C1450" t="n">
+        <v>-4481</v>
+      </c>
+      <c r="D1450" t="n">
+        <v>65892</v>
+      </c>
+      <c r="E1450" t="n">
+        <v>61411</v>
+      </c>
+      <c r="F1450" t="n">
+        <v>139651</v>
+      </c>
+      <c r="G1450" t="n">
+        <v>84871</v>
+      </c>
+      <c r="H1450" t="n">
+        <v>229516</v>
+      </c>
+      <c r="I1450" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="J1450" t="n">
+        <v>-249</v>
+      </c>
+      <c r="K1450" t="n">
+        <v>9000</v>
+      </c>
+      <c r="L1450" t="n">
+        <v>4994</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>

<commit_message>
pylintrc and small changes
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -394,7 +394,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1456"/>
+  <dimension ref="A1:L1468"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1004" activePane="bottomRight" state="frozenSplit"/>
@@ -52372,6 +52372,486 @@
         <v>5479</v>
       </c>
     </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>2023-09-20</t>
+        </is>
+      </c>
+      <c r="B1457" t="n">
+        <v>67942</v>
+      </c>
+      <c r="C1457" t="n">
+        <v>10556</v>
+      </c>
+      <c r="D1457" t="n">
+        <v>66962</v>
+      </c>
+      <c r="E1457" t="n">
+        <v>77518</v>
+      </c>
+      <c r="F1457" t="n">
+        <v>145460</v>
+      </c>
+      <c r="G1457" t="n">
+        <v>91879</v>
+      </c>
+      <c r="H1457" t="n">
+        <v>242776</v>
+      </c>
+      <c r="I1457" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="J1457" t="n">
+        <v>14871</v>
+      </c>
+      <c r="K1457" t="n">
+        <v>9000</v>
+      </c>
+      <c r="L1457" t="n">
+        <v>5437</v>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>2023-09-21</t>
+        </is>
+      </c>
+      <c r="B1458" t="n">
+        <v>67942</v>
+      </c>
+      <c r="C1458" t="n">
+        <v>10547</v>
+      </c>
+      <c r="D1458" t="n">
+        <v>65855</v>
+      </c>
+      <c r="E1458" t="n">
+        <v>76402</v>
+      </c>
+      <c r="F1458" t="n">
+        <v>144344</v>
+      </c>
+      <c r="G1458" t="n">
+        <v>91737</v>
+      </c>
+      <c r="H1458" t="n">
+        <v>241419</v>
+      </c>
+      <c r="I1458" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="J1458" t="n">
+        <v>14862</v>
+      </c>
+      <c r="K1458" t="n">
+        <v>9000</v>
+      </c>
+      <c r="L1458" t="n">
+        <v>5338</v>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>2023-09-28</t>
+        </is>
+      </c>
+      <c r="B1459" t="n">
+        <v>67942</v>
+      </c>
+      <c r="C1459" t="n">
+        <v>10609</v>
+      </c>
+      <c r="D1459" t="n">
+        <v>65213</v>
+      </c>
+      <c r="E1459" t="n">
+        <v>75822</v>
+      </c>
+      <c r="F1459" t="n">
+        <v>143764</v>
+      </c>
+      <c r="G1459" t="n">
+        <v>91585</v>
+      </c>
+      <c r="H1459" t="n">
+        <v>240695</v>
+      </c>
+      <c r="I1459" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="J1459" t="n">
+        <v>14872</v>
+      </c>
+      <c r="K1459" t="n">
+        <v>9000</v>
+      </c>
+      <c r="L1459" t="n">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>2023-10-06</t>
+        </is>
+      </c>
+      <c r="B1460" t="n">
+        <v>68021</v>
+      </c>
+      <c r="C1460" t="n">
+        <v>10603</v>
+      </c>
+      <c r="D1460" t="n">
+        <v>67353</v>
+      </c>
+      <c r="E1460" t="n">
+        <v>77956</v>
+      </c>
+      <c r="F1460" t="n">
+        <v>145977</v>
+      </c>
+      <c r="G1460" t="n">
+        <v>91619</v>
+      </c>
+      <c r="H1460" t="n">
+        <v>242956</v>
+      </c>
+      <c r="I1460" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="J1460" t="n">
+        <v>14891</v>
+      </c>
+      <c r="K1460" t="n">
+        <v>9000</v>
+      </c>
+      <c r="L1460" t="n">
+        <v>5360</v>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>2023-10-07</t>
+        </is>
+      </c>
+      <c r="B1461" t="n">
+        <v>68021</v>
+      </c>
+      <c r="C1461" t="n">
+        <v>10603</v>
+      </c>
+      <c r="D1461" t="n">
+        <v>67396</v>
+      </c>
+      <c r="E1461" t="n">
+        <v>77999</v>
+      </c>
+      <c r="F1461" t="n">
+        <v>146020</v>
+      </c>
+      <c r="G1461" t="n">
+        <v>91619</v>
+      </c>
+      <c r="H1461" t="n">
+        <v>242999</v>
+      </c>
+      <c r="I1461" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="J1461" t="n">
+        <v>14893</v>
+      </c>
+      <c r="K1461" t="n">
+        <v>9000</v>
+      </c>
+      <c r="L1461" t="n">
+        <v>5360</v>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>2023-10-12</t>
+        </is>
+      </c>
+      <c r="B1462" t="n">
+        <v>68021</v>
+      </c>
+      <c r="C1462" t="n">
+        <v>10636</v>
+      </c>
+      <c r="D1462" t="n">
+        <v>68551</v>
+      </c>
+      <c r="E1462" t="n">
+        <v>79187</v>
+      </c>
+      <c r="F1462" t="n">
+        <v>147208</v>
+      </c>
+      <c r="G1462" t="n">
+        <v>91834</v>
+      </c>
+      <c r="H1462" t="n">
+        <v>244580</v>
+      </c>
+      <c r="I1462" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="J1462" t="n">
+        <v>14863</v>
+      </c>
+      <c r="K1462" t="n">
+        <v>9000</v>
+      </c>
+      <c r="L1462" t="n">
+        <v>5538</v>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>2023-10-14</t>
+        </is>
+      </c>
+      <c r="B1463" t="n">
+        <v>68021</v>
+      </c>
+      <c r="C1463" t="n">
+        <v>10647</v>
+      </c>
+      <c r="D1463" t="n">
+        <v>67521</v>
+      </c>
+      <c r="E1463" t="n">
+        <v>78168</v>
+      </c>
+      <c r="F1463" t="n">
+        <v>146189</v>
+      </c>
+      <c r="G1463" t="n">
+        <v>91751</v>
+      </c>
+      <c r="H1463" t="n">
+        <v>243418</v>
+      </c>
+      <c r="I1463" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="J1463" t="n">
+        <v>14870</v>
+      </c>
+      <c r="K1463" t="n">
+        <v>9000</v>
+      </c>
+      <c r="L1463" t="n">
+        <v>5478</v>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>2023-10-25</t>
+        </is>
+      </c>
+      <c r="B1464" t="n">
+        <v>68021</v>
+      </c>
+      <c r="C1464" t="n">
+        <v>10630</v>
+      </c>
+      <c r="D1464" t="n">
+        <v>63996</v>
+      </c>
+      <c r="E1464" t="n">
+        <v>74626</v>
+      </c>
+      <c r="F1464" t="n">
+        <v>142647</v>
+      </c>
+      <c r="G1464" t="n">
+        <v>91319</v>
+      </c>
+      <c r="H1464" t="n">
+        <v>239297</v>
+      </c>
+      <c r="I1464" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="J1464" t="n">
+        <v>15021</v>
+      </c>
+      <c r="K1464" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L1464" t="n">
+        <v>5331</v>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>2023-10-26</t>
+        </is>
+      </c>
+      <c r="B1465" t="n">
+        <v>68021</v>
+      </c>
+      <c r="C1465" t="n">
+        <v>10620</v>
+      </c>
+      <c r="D1465" t="n">
+        <v>62968</v>
+      </c>
+      <c r="E1465" t="n">
+        <v>73588</v>
+      </c>
+      <c r="F1465" t="n">
+        <v>141609</v>
+      </c>
+      <c r="G1465" t="n">
+        <v>91198</v>
+      </c>
+      <c r="H1465" t="n">
+        <v>238046</v>
+      </c>
+      <c r="I1465" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="J1465" t="n">
+        <v>15008</v>
+      </c>
+      <c r="K1465" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L1465" t="n">
+        <v>5239</v>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>2023-11-03</t>
+        </is>
+      </c>
+      <c r="B1466" t="n">
+        <v>62855</v>
+      </c>
+      <c r="C1466" t="n">
+        <v>10606</v>
+      </c>
+      <c r="D1466" t="n">
+        <v>69150</v>
+      </c>
+      <c r="E1466" t="n">
+        <v>79756</v>
+      </c>
+      <c r="F1466" t="n">
+        <v>142611</v>
+      </c>
+      <c r="G1466" t="n">
+        <v>86865</v>
+      </c>
+      <c r="H1466" t="n">
+        <v>234859</v>
+      </c>
+      <c r="I1466" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="J1466" t="n">
+        <v>13576</v>
+      </c>
+      <c r="K1466" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L1466" t="n">
+        <v>5383</v>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>2023-11-04</t>
+        </is>
+      </c>
+      <c r="B1467" t="n">
+        <v>62855</v>
+      </c>
+      <c r="C1467" t="n">
+        <v>10606</v>
+      </c>
+      <c r="D1467" t="n">
+        <v>71097</v>
+      </c>
+      <c r="E1467" t="n">
+        <v>81703</v>
+      </c>
+      <c r="F1467" t="n">
+        <v>144558</v>
+      </c>
+      <c r="G1467" t="n">
+        <v>88865</v>
+      </c>
+      <c r="H1467" t="n">
+        <v>238808</v>
+      </c>
+      <c r="I1467" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="J1467" t="n">
+        <v>13583</v>
+      </c>
+      <c r="K1467" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L1467" t="n">
+        <v>5385</v>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>2023-11-11</t>
+        </is>
+      </c>
+      <c r="B1468" t="n">
+        <v>75685</v>
+      </c>
+      <c r="C1468" t="n">
+        <v>-4372</v>
+      </c>
+      <c r="D1468" t="n">
+        <v>69205</v>
+      </c>
+      <c r="E1468" t="n">
+        <v>64833</v>
+      </c>
+      <c r="F1468" t="n">
+        <v>140518</v>
+      </c>
+      <c r="G1468" t="n">
+        <v>89271</v>
+      </c>
+      <c r="H1468" t="n">
+        <v>235231</v>
+      </c>
+      <c r="I1468" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="J1468" t="n">
+        <v>-1251</v>
+      </c>
+      <c r="K1468" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L1468" t="n">
+        <v>5442</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>

<commit_message>
chore: Update EVERAUS_VOLAKIRI constant in Valme.py
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -54182,28 +54182,28 @@
         <v>52185</v>
       </c>
       <c r="C1502" t="n">
-        <v>-10000</v>
+        <v>-4441</v>
       </c>
       <c r="D1502" t="n">
-        <v>87501</v>
+        <v>87500</v>
       </c>
       <c r="E1502" t="n">
-        <v>77501</v>
+        <v>83059</v>
       </c>
       <c r="F1502" t="n">
-        <v>129686</v>
+        <v>135244</v>
       </c>
       <c r="G1502" t="n">
-        <v>78557</v>
+        <v>77520</v>
       </c>
       <c r="H1502" t="n">
-        <v>217022</v>
+        <v>221543</v>
       </c>
       <c r="I1502" t="n">
         <v>91.13</v>
       </c>
       <c r="J1502" t="n">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="K1502" t="n">
         <v>4400</v>

</xml_diff>

<commit_message>
assets plot changed from static to dynamic
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -54185,31 +54185,31 @@
         <v>-4454</v>
       </c>
       <c r="D1502" t="n">
-        <v>87586</v>
+        <v>87389</v>
       </c>
       <c r="E1502" t="n">
-        <v>83132</v>
+        <v>82935</v>
       </c>
       <c r="F1502" t="n">
-        <v>135317</v>
+        <v>135120</v>
       </c>
       <c r="G1502" t="n">
         <v>78554</v>
       </c>
       <c r="H1502" t="n">
-        <v>222660</v>
+        <v>222461</v>
       </c>
       <c r="I1502" t="n">
         <v>91.13</v>
       </c>
       <c r="J1502" t="n">
-        <v>873</v>
+        <v>862</v>
       </c>
       <c r="K1502" t="n">
         <v>4400</v>
       </c>
       <c r="L1502" t="n">
-        <v>8789</v>
+        <v>8787</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock price getting logic seperated
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -394,7 +394,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1502"/>
+  <dimension ref="A1:L1503"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1004" activePane="bottomRight" state="frozenSplit"/>
@@ -54212,6 +54212,46 @@
         <v>8787</v>
       </c>
     </row>
+    <row r="1503">
+      <c r="A1503" t="inlineStr">
+        <is>
+          <t>2024-07-17</t>
+        </is>
+      </c>
+      <c r="B1503" t="n">
+        <v>52185</v>
+      </c>
+      <c r="C1503" t="n">
+        <v>-4771</v>
+      </c>
+      <c r="D1503" t="n">
+        <v>86137</v>
+      </c>
+      <c r="E1503" t="n">
+        <v>81366</v>
+      </c>
+      <c r="F1503" t="n">
+        <v>133551</v>
+      </c>
+      <c r="G1503" t="n">
+        <v>77906</v>
+      </c>
+      <c r="H1503" t="n">
+        <v>220089</v>
+      </c>
+      <c r="I1503" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="J1503" t="n">
+        <v>-135</v>
+      </c>
+      <c r="K1503" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1503" t="n">
+        <v>8632</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>

<commit_message>
send email and email body moved to new utils file
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -394,7 +394,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1504"/>
+  <dimension ref="A1:L1505"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1004" activePane="bottomRight" state="frozenSplit"/>
@@ -54265,31 +54265,71 @@
         <v>-4468</v>
       </c>
       <c r="D1504" t="n">
-        <v>84006</v>
+        <v>83997</v>
       </c>
       <c r="E1504" t="n">
-        <v>79538</v>
+        <v>79529</v>
       </c>
       <c r="F1504" t="n">
-        <v>131723</v>
+        <v>131714</v>
       </c>
       <c r="G1504" t="n">
         <v>79040</v>
       </c>
       <c r="H1504" t="n">
-        <v>219259</v>
+        <v>219251</v>
       </c>
       <c r="I1504" t="n">
         <v>91.13</v>
       </c>
       <c r="J1504" t="n">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="K1504" t="n">
         <v>4400</v>
       </c>
       <c r="L1504" t="n">
-        <v>8496</v>
+        <v>8497</v>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" t="inlineStr">
+        <is>
+          <t>2024-08-03</t>
+        </is>
+      </c>
+      <c r="B1505" t="n">
+        <v>52185</v>
+      </c>
+      <c r="C1505" t="n">
+        <v>-4471</v>
+      </c>
+      <c r="D1505" t="n">
+        <v>79440</v>
+      </c>
+      <c r="E1505" t="n">
+        <v>74969</v>
+      </c>
+      <c r="F1505" t="n">
+        <v>127154</v>
+      </c>
+      <c r="G1505" t="n">
+        <v>78085</v>
+      </c>
+      <c r="H1505" t="n">
+        <v>213223</v>
+      </c>
+      <c r="I1505" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="J1505" t="n">
+        <v>741</v>
+      </c>
+      <c r="K1505" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1505" t="n">
+        <v>7984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
file paths and NAs paths moved to utils from main script run
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -394,7 +394,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1506"/>
+  <dimension ref="A1:L1507"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1004" activePane="bottomRight" state="frozenSplit"/>
@@ -54345,31 +54345,71 @@
         <v>-4471</v>
       </c>
       <c r="D1506" t="n">
-        <v>79439</v>
+        <v>79436</v>
       </c>
       <c r="E1506" t="n">
-        <v>74968</v>
+        <v>74965</v>
       </c>
       <c r="F1506" t="n">
-        <v>127153</v>
+        <v>127150</v>
       </c>
       <c r="G1506" t="n">
         <v>78394</v>
       </c>
       <c r="H1506" t="n">
-        <v>213691</v>
+        <v>213686</v>
       </c>
       <c r="I1506" t="n">
         <v>91.13</v>
       </c>
       <c r="J1506" t="n">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="K1506" t="n">
         <v>4400</v>
       </c>
       <c r="L1506" t="n">
-        <v>8144</v>
+        <v>8142</v>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr">
+        <is>
+          <t>2024-08-18</t>
+        </is>
+      </c>
+      <c r="B1507" t="n">
+        <v>51185</v>
+      </c>
+      <c r="C1507" t="n">
+        <v>-4534</v>
+      </c>
+      <c r="D1507" t="n">
+        <v>81153</v>
+      </c>
+      <c r="E1507" t="n">
+        <v>76619</v>
+      </c>
+      <c r="F1507" t="n">
+        <v>127804</v>
+      </c>
+      <c r="G1507" t="n">
+        <v>78073</v>
+      </c>
+      <c r="H1507" t="n">
+        <v>214310</v>
+      </c>
+      <c r="I1507" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="J1507" t="n">
+        <v>682</v>
+      </c>
+      <c r="K1507" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1507" t="n">
+        <v>8433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed copy logic to support win and mac os, changed terminal to file logic. Added loguru to some parts of the code
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -394,7 +394,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1507"/>
+  <dimension ref="A1:L1508"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1004" activePane="bottomRight" state="frozenSplit"/>
@@ -54412,6 +54412,46 @@
         <v>8434</v>
       </c>
     </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr">
+        <is>
+          <t>2024-08-24</t>
+        </is>
+      </c>
+      <c r="B1508" t="n">
+        <v>51185</v>
+      </c>
+      <c r="C1508" t="n">
+        <v>-10000</v>
+      </c>
+      <c r="D1508" t="n">
+        <v>80223</v>
+      </c>
+      <c r="E1508" t="n">
+        <v>70223</v>
+      </c>
+      <c r="F1508" t="n">
+        <v>121408</v>
+      </c>
+      <c r="G1508" t="n">
+        <v>71034</v>
+      </c>
+      <c r="H1508" t="n">
+        <v>199945</v>
+      </c>
+      <c r="I1508" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="J1508" t="n">
+        <v>745</v>
+      </c>
+      <c r="K1508" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1508" t="n">
+        <v>7503</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>

<commit_message>
small changes and data update
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -394,7 +394,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1508"/>
+  <dimension ref="A1:L1509"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1004" activePane="bottomRight" state="frozenSplit"/>
@@ -54452,6 +54452,46 @@
         <v>7503</v>
       </c>
     </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr">
+        <is>
+          <t>2024-08-31</t>
+        </is>
+      </c>
+      <c r="B1509" t="n">
+        <v>51185</v>
+      </c>
+      <c r="C1509" t="n">
+        <v>-6663</v>
+      </c>
+      <c r="D1509" t="n">
+        <v>81694</v>
+      </c>
+      <c r="E1509" t="n">
+        <v>75031</v>
+      </c>
+      <c r="F1509" t="n">
+        <v>126216</v>
+      </c>
+      <c r="G1509" t="n">
+        <v>78384</v>
+      </c>
+      <c r="H1509" t="n">
+        <v>213158</v>
+      </c>
+      <c r="I1509" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="J1509" t="n">
+        <v>873</v>
+      </c>
+      <c r="K1509" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1509" t="n">
+        <v>8558</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>

<commit_message>
family prints moved to sperate func
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -54462,34 +54462,34 @@
         <v>51185</v>
       </c>
       <c r="C1509" t="n">
-        <v>-6663</v>
+        <v>-4567</v>
       </c>
       <c r="D1509" t="n">
-        <v>81694</v>
+        <v>81691</v>
       </c>
       <c r="E1509" t="n">
-        <v>75031</v>
+        <v>77124</v>
       </c>
       <c r="F1509" t="n">
-        <v>126216</v>
+        <v>128309</v>
       </c>
       <c r="G1509" t="n">
         <v>78384</v>
       </c>
       <c r="H1509" t="n">
-        <v>213158</v>
+        <v>215110</v>
       </c>
       <c r="I1509" t="n">
         <v>91.13</v>
       </c>
       <c r="J1509" t="n">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="K1509" t="n">
         <v>4400</v>
       </c>
       <c r="L1509" t="n">
-        <v>8558</v>
+        <v>8417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small general and config changes
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -336,7 +336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L1510"/>
+  <dimension ref="A1:L1511"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1497" activePane="bottomRight" state="frozen"/>
@@ -54475,6 +54475,46 @@
         <v>8182</v>
       </c>
     </row>
+    <row r="1511">
+      <c r="A1511" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-07</t>
+        </is>
+      </c>
+      <c r="B1511" s="2" t="n">
+        <v>51185</v>
+      </c>
+      <c r="C1511" s="2" t="n">
+        <v>-4191</v>
+      </c>
+      <c r="D1511" s="2" t="n">
+        <v>80204</v>
+      </c>
+      <c r="E1511" s="2" t="n">
+        <v>76013</v>
+      </c>
+      <c r="F1511" s="2" t="n">
+        <v>127198</v>
+      </c>
+      <c r="G1511" s="2" t="n">
+        <v>79206</v>
+      </c>
+      <c r="H1511" s="2" t="n">
+        <v>215351</v>
+      </c>
+      <c r="I1511" s="2" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="J1511" s="2" t="n">
+        <v>778</v>
+      </c>
+      <c r="K1511" s="2" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1511" s="2" t="n">
+        <v>8947</v>
+      </c>
+    </row>
     <row r="1048576" ht="12.8" customHeight="1" s="3"/>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
added twilio send email to replace Synology NAS email send
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -336,7 +336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L1511"/>
+  <dimension ref="A1:L1513"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1497" activePane="bottomRight" state="frozen"/>
@@ -54515,6 +54515,86 @@
         <v>8947</v>
       </c>
     </row>
+    <row r="1512">
+      <c r="A1512" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="B1512" s="2" t="n">
+        <v>51185</v>
+      </c>
+      <c r="C1512" s="2" t="n">
+        <v>-4141</v>
+      </c>
+      <c r="D1512" s="2" t="n">
+        <v>80299</v>
+      </c>
+      <c r="E1512" s="2" t="n">
+        <v>76158</v>
+      </c>
+      <c r="F1512" s="2" t="n">
+        <v>127343</v>
+      </c>
+      <c r="G1512" s="2" t="n">
+        <v>78153</v>
+      </c>
+      <c r="H1512" s="2" t="n">
+        <v>213987</v>
+      </c>
+      <c r="I1512" s="2" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="J1512" s="2" t="n">
+        <v>847</v>
+      </c>
+      <c r="K1512" s="2" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1512" s="2" t="n">
+        <v>8491</v>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="B1513" s="2" t="n">
+        <v>51185</v>
+      </c>
+      <c r="C1513" s="2" t="n">
+        <v>-4155</v>
+      </c>
+      <c r="D1513" s="2" t="n">
+        <v>83131</v>
+      </c>
+      <c r="E1513" s="2" t="n">
+        <v>78976</v>
+      </c>
+      <c r="F1513" s="2" t="n">
+        <v>130161</v>
+      </c>
+      <c r="G1513" s="2" t="n">
+        <v>78481</v>
+      </c>
+      <c r="H1513" s="2" t="n">
+        <v>217119</v>
+      </c>
+      <c r="I1513" s="2" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="J1513" s="2" t="n">
+        <v>934</v>
+      </c>
+      <c r="K1513" s="2" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1513" s="2" t="n">
+        <v>8477</v>
+      </c>
+    </row>
     <row r="1048576" ht="12.8" customHeight="1" s="3"/>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
removed yfinance, to finhhub and to use yahoo selenium if nothing else works. Other smaller changes
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -54765,34 +54765,34 @@
         <v>51185</v>
       </c>
       <c r="C1518" s="2" t="n">
-        <v>-9575</v>
+        <v>-4437</v>
       </c>
       <c r="D1518" s="2" t="n">
-        <v>84736</v>
+        <v>75166</v>
       </c>
       <c r="E1518" s="2" t="n">
-        <v>75161</v>
+        <v>70729</v>
       </c>
       <c r="F1518" s="2" t="n">
-        <v>126346</v>
+        <v>121914</v>
       </c>
       <c r="G1518" s="2" t="n">
-        <v>72275</v>
+        <v>79250</v>
       </c>
       <c r="H1518" s="2" t="n">
-        <v>207029</v>
+        <v>210193</v>
       </c>
       <c r="I1518" s="2" t="n">
         <v>91.13</v>
       </c>
       <c r="J1518" s="2" t="n">
-        <v>1384</v>
+        <v>1388</v>
       </c>
       <c r="K1518" s="2" t="n">
         <v>4400</v>
       </c>
       <c r="L1518" s="2" t="n">
-        <v>8408</v>
+        <v>9029</v>
       </c>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="3"/>

</xml_diff>

<commit_message>
to reduce errors with chorme Driver
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -336,7 +336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L1518"/>
+  <dimension ref="A1:L1520"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1497" activePane="bottomRight" state="frozen"/>
@@ -54795,6 +54795,86 @@
         <v>9029</v>
       </c>
     </row>
+    <row r="1519">
+      <c r="A1519" s="2" t="inlineStr">
+        <is>
+          <t>2024-10-25</t>
+        </is>
+      </c>
+      <c r="B1519" s="2" t="n">
+        <v>93532.5</v>
+      </c>
+      <c r="C1519" s="2" t="n">
+        <v>-4422</v>
+      </c>
+      <c r="D1519" s="2" t="n">
+        <v>75390</v>
+      </c>
+      <c r="E1519" s="2" t="n">
+        <v>70968</v>
+      </c>
+      <c r="F1519" s="2" t="n">
+        <v>164500.5</v>
+      </c>
+      <c r="G1519" s="2" t="n">
+        <v>121644</v>
+      </c>
+      <c r="H1519" s="2" t="n">
+        <v>295464.5</v>
+      </c>
+      <c r="I1519" s="2" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="J1519" s="2" t="n">
+        <v>1392</v>
+      </c>
+      <c r="K1519" s="2" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1519" s="2" t="n">
+        <v>9320</v>
+      </c>
+    </row>
+    <row r="1520">
+      <c r="A1520" s="2" t="inlineStr">
+        <is>
+          <t>2024-10-27</t>
+        </is>
+      </c>
+      <c r="B1520" s="2" t="n">
+        <v>93532.5</v>
+      </c>
+      <c r="C1520" s="2" t="n">
+        <v>-3996</v>
+      </c>
+      <c r="D1520" s="2" t="n">
+        <v>75991</v>
+      </c>
+      <c r="E1520" s="2" t="n">
+        <v>71995</v>
+      </c>
+      <c r="F1520" s="2" t="n">
+        <v>165527.5</v>
+      </c>
+      <c r="G1520" s="2" t="n">
+        <v>121757</v>
+      </c>
+      <c r="H1520" s="2" t="n">
+        <v>296676.5</v>
+      </c>
+      <c r="I1520" s="2" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="J1520" s="2" t="n">
+        <v>1387</v>
+      </c>
+      <c r="K1520" s="2" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1520" s="2" t="n">
+        <v>9392</v>
+      </c>
+    </row>
     <row r="1048576" ht="12.8" customHeight="1" s="3"/>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
google scraping and chromedriver changes
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -54845,34 +54845,34 @@
         <v>93532.5</v>
       </c>
       <c r="C1520" s="2" t="n">
-        <v>-3996</v>
+        <v>-4422</v>
       </c>
       <c r="D1520" s="2" t="n">
-        <v>75991</v>
+        <v>85863</v>
       </c>
       <c r="E1520" s="2" t="n">
-        <v>71995</v>
+        <v>81441</v>
       </c>
       <c r="F1520" s="2" t="n">
-        <v>165527.5</v>
+        <v>174973.5</v>
       </c>
       <c r="G1520" s="2" t="n">
         <v>121757</v>
       </c>
       <c r="H1520" s="2" t="n">
-        <v>296676.5</v>
+        <v>305603.5</v>
       </c>
       <c r="I1520" s="2" t="n">
         <v>91.13</v>
       </c>
       <c r="J1520" s="2" t="n">
-        <v>1387</v>
+        <v>1383</v>
       </c>
       <c r="K1520" s="2" t="n">
         <v>4400</v>
       </c>
       <c r="L1520" s="2" t="n">
-        <v>9392</v>
+        <v>8873</v>
       </c>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="3"/>

</xml_diff>

<commit_message>
get_default_user_agent added to support linux better for price webscrape
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -336,7 +336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L1520"/>
+  <dimension ref="A1:L1521"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1497" activePane="bottomRight" state="frozen"/>
@@ -54875,6 +54875,46 @@
         <v>8873</v>
       </c>
     </row>
+    <row r="1521">
+      <c r="A1521" s="2" t="inlineStr">
+        <is>
+          <t>2024-10-31</t>
+        </is>
+      </c>
+      <c r="B1521" s="2" t="n">
+        <v>93532.5</v>
+      </c>
+      <c r="C1521" s="2" t="n">
+        <v>-4102</v>
+      </c>
+      <c r="D1521" s="2" t="n">
+        <v>85687</v>
+      </c>
+      <c r="E1521" s="2" t="n">
+        <v>81585</v>
+      </c>
+      <c r="F1521" s="2" t="n">
+        <v>175117.5</v>
+      </c>
+      <c r="G1521" s="2" t="n">
+        <v>121307</v>
+      </c>
+      <c r="H1521" s="2" t="n">
+        <v>305654.5</v>
+      </c>
+      <c r="I1521" s="2" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="J1521" s="2" t="n">
+        <v>1469</v>
+      </c>
+      <c r="K1521" s="2" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1521" s="2" t="n">
+        <v>9230</v>
+      </c>
+    </row>
     <row r="1048576" ht="12.8" customHeight="1" s="3"/>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
added yfinance back as this works again and is much more reliable
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -336,7 +336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L1522"/>
+  <dimension ref="A1:L1523"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1497" activePane="bottomRight" state="frozen"/>
@@ -54955,6 +54955,46 @@
         <v>486</v>
       </c>
     </row>
+    <row r="1523">
+      <c r="A1523" s="2" t="inlineStr">
+        <is>
+          <t>2024-12-01</t>
+        </is>
+      </c>
+      <c r="B1523" s="2" t="n">
+        <v>86016</v>
+      </c>
+      <c r="C1523" s="2" t="n">
+        <v>-3381</v>
+      </c>
+      <c r="D1523" s="2" t="n">
+        <v>91635</v>
+      </c>
+      <c r="E1523" s="2" t="n">
+        <v>88254</v>
+      </c>
+      <c r="F1523" s="2" t="n">
+        <v>174270</v>
+      </c>
+      <c r="G1523" s="2" t="n">
+        <v>113289</v>
+      </c>
+      <c r="H1523" s="2" t="n">
+        <v>299067</v>
+      </c>
+      <c r="I1523" s="2" t="n">
+        <v>100.22</v>
+      </c>
+      <c r="J1523" s="2" t="n">
+        <v>2028</v>
+      </c>
+      <c r="K1523" s="2" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1523" s="2" t="n">
+        <v>11508</v>
+      </c>
+    </row>
     <row r="1048576" ht="12.8" customHeight="1" s="3"/>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
crypto valme to zero
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -54968,31 +54968,31 @@
         <v>-3381</v>
       </c>
       <c r="D1523" s="2" t="n">
-        <v>91635</v>
+        <v>91638</v>
       </c>
       <c r="E1523" s="2" t="n">
-        <v>88254</v>
+        <v>88257</v>
       </c>
       <c r="F1523" s="2" t="n">
-        <v>174270</v>
+        <v>174273</v>
       </c>
       <c r="G1523" s="2" t="n">
         <v>113289</v>
       </c>
       <c r="H1523" s="2" t="n">
-        <v>299067</v>
+        <v>299071</v>
       </c>
       <c r="I1523" s="2" t="n">
         <v>100.22</v>
       </c>
       <c r="J1523" s="2" t="n">
-        <v>2028</v>
+        <v>2031</v>
       </c>
       <c r="K1523" s="2" t="n">
         <v>4400</v>
       </c>
       <c r="L1523" s="2" t="n">
-        <v>11508</v>
+        <v>11509</v>
       </c>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="3"/>

</xml_diff>

<commit_message>
change to use pydantic setttings for config
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -332,7 +332,7 @@
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L1525"/>
+  <dimension ref="A1:L1526"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" zoomScale="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -55068,6 +55068,46 @@
         <v>10290</v>
       </c>
     </row>
+    <row r="1526">
+      <c r="A1526" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="B1526" t="n">
+        <v>86016</v>
+      </c>
+      <c r="C1526" t="n">
+        <v>-2726</v>
+      </c>
+      <c r="D1526" t="n">
+        <v>105344</v>
+      </c>
+      <c r="E1526" t="n">
+        <v>102618</v>
+      </c>
+      <c r="F1526" t="n">
+        <v>188634</v>
+      </c>
+      <c r="G1526" t="n">
+        <v>124844</v>
+      </c>
+      <c r="H1526" t="n">
+        <v>324118</v>
+      </c>
+      <c r="I1526" t="n">
+        <v>109.31</v>
+      </c>
+      <c r="J1526" t="n">
+        <v>-426</v>
+      </c>
+      <c r="K1526" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1526" t="n">
+        <v>10640</v>
+      </c>
+    </row>
     <row r="1048576" ht="12.8" customHeight="1" s="2"/>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
made init changes and created portfolio owners dir
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -55278,22 +55278,22 @@
         <v>86016</v>
       </c>
       <c r="C1531" t="n">
-        <v>-3544</v>
+        <v>-3540</v>
       </c>
       <c r="D1531" t="n">
-        <v>96989</v>
+        <v>97012</v>
       </c>
       <c r="E1531" t="n">
-        <v>93445</v>
+        <v>93472</v>
       </c>
       <c r="F1531" t="n">
-        <v>179461</v>
+        <v>179488</v>
       </c>
       <c r="G1531" t="n">
-        <v>120283</v>
+        <v>120304</v>
       </c>
       <c r="H1531" t="n">
-        <v>308929</v>
+        <v>308986</v>
       </c>
       <c r="I1531" t="n">
         <v>109.31</v>
@@ -55305,7 +55305,7 @@
         <v>4400</v>
       </c>
       <c r="L1531" t="n">
-        <v>9185</v>
+        <v>9194</v>
       </c>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="2"/>

</xml_diff>

<commit_message>
logging added and stock prices validatsions
</commit_message>
<xml_diff>
--- a/Portfell.xlsx
+++ b/Portfell.xlsx
@@ -332,7 +332,7 @@
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L1531"/>
+  <dimension ref="A1:L1532"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" zoomScale="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -55308,6 +55308,46 @@
         <v>9206</v>
       </c>
     </row>
+    <row r="1532">
+      <c r="A1532" t="inlineStr">
+        <is>
+          <t>2025-03-16</t>
+        </is>
+      </c>
+      <c r="B1532" t="n">
+        <v>86016</v>
+      </c>
+      <c r="C1532" t="n">
+        <v>-3530</v>
+      </c>
+      <c r="D1532" t="n">
+        <v>98088</v>
+      </c>
+      <c r="E1532" t="n">
+        <v>94558</v>
+      </c>
+      <c r="F1532" t="n">
+        <v>180574</v>
+      </c>
+      <c r="G1532" t="n">
+        <v>120421</v>
+      </c>
+      <c r="H1532" t="n">
+        <v>310268</v>
+      </c>
+      <c r="I1532" t="n">
+        <v>109.31</v>
+      </c>
+      <c r="J1532" t="n">
+        <v>203</v>
+      </c>
+      <c r="K1532" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1532" t="n">
+        <v>9273</v>
+      </c>
+    </row>
     <row r="1048576" ht="12.8" customHeight="1" s="2"/>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>